<commit_message>
Added Gewichtung and Diagramm for Nutzwertanalyse, Edited Mail texte, Modified Template for Nutzwertanalyse
</commit_message>
<xml_diff>
--- a/ROOT/5. SCM-Nutzwertanalyse.xlsx
+++ b/ROOT/5. SCM-Nutzwertanalyse.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anouar\PycharmProjects\scm\ROOT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emil/git/scm/ROOT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD84ADEA-E65A-40C2-B612-F4E07F377EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E300E5-03F1-5F43-A4A9-418BDD4EE52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2D5E02D-B118-4755-A46F-9D78F33943BD}"/>
+    <workbookView xWindow="160" yWindow="940" windowWidth="33900" windowHeight="21060" xr2:uid="{A2D5E02D-B118-4755-A46F-9D78F33943BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -154,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +167,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -600,6 +607,1049 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Lieferanten im Vergleich</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nutzwerte</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="84000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001B-BD6E-9246-A05D-08317981580C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$31:$V$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001A-BD6E-9246-A05D-08317981580C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="41"/>
+        <c:axId val="2084127056"/>
+        <c:axId val="1232244960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2084127056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1232244960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1232244960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Nutzwert</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2084127056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="68000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:lin ang="5400000" scaled="1"/>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="204">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200">
+      <a:effectLst/>
+    </cs:defRPr>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="68000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="84000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr kern="1200">
+      <a:effectLst/>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Nutzwerte">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74077EE3-33DF-8C7D-C774-71A3C80B23AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -917,20 +1967,56 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0BB4E8A0-3D59-8849-9980-91919DCEE009}">
+  <we:reference id="ccf3b6fe-92cf-4884-a902-238ad9305f9a" version="1.0.0.3" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences>
+    <we:reference id="WA200002252" version="1.0.0.3" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_WISE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_WISEPRICE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_WISEFUNDS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_WISEOPTIONS</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{0858819E-0033-43BF-8937-05EC82904868}">
+      <we:backgroundApp state="1" runtimeId="Taskpane.Url"/>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2552A7B-C0EC-47EF-B133-BEE4AA3F3818}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -946,7 +2032,7 @@
       </c>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
       <c r="B2" s="29"/>
       <c r="C2" s="13" t="s">
@@ -962,7 +2048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>6</v>
       </c>
@@ -972,12 +2058,12 @@
       <c r="E3" s="26"/>
       <c r="F3" s="27"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="8">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2">
@@ -990,12 +2076,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="9">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2">
@@ -1008,12 +2094,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="9">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2">
@@ -1026,12 +2112,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="9">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2">
@@ -1044,12 +2130,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="7">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="2">
@@ -1062,7 +2148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>7</v>
       </c>
@@ -1072,12 +2158,12 @@
       <c r="E9" s="26"/>
       <c r="F9" s="27"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2">
@@ -1090,12 +2176,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="9">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2">
@@ -1108,12 +2194,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="9">
-        <v>1</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2">
@@ -1126,12 +2212,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="12">
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="2">
@@ -1144,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>12</v>
       </c>
@@ -1154,12 +2240,12 @@
       <c r="E14" s="26"/>
       <c r="F14" s="27"/>
     </row>
-    <row r="15" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="8">
-        <v>1</v>
+        <v>0.09</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2">
@@ -1172,12 +2258,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>1</v>
+        <v>0.09</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="2">
@@ -1190,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>15</v>
       </c>
@@ -1200,12 +2286,12 @@
       <c r="E17" s="26"/>
       <c r="F17" s="27"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="8">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="2">
@@ -1218,12 +2304,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2">
@@ -1236,12 +2322,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>1</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="2">
@@ -1254,12 +2340,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="5">
-        <v>1</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="2">
@@ -1272,12 +2358,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="7">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="2">
@@ -1290,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>21</v>
       </c>
@@ -1300,12 +2386,12 @@
       <c r="E23" s="26"/>
       <c r="F23" s="27"/>
     </row>
-    <row r="24" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="17">
-        <v>1</v>
+        <v>0.06</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="2">
@@ -1318,16 +2404,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="9">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="2">
-        <f>B25*C25</f>
         <v>0</v>
       </c>
       <c r="E25" s="1"/>
@@ -1336,12 +2421,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="12">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="2">
@@ -1354,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>25</v>
       </c>
@@ -1364,12 +2449,12 @@
       <c r="E27" s="26"/>
       <c r="F27" s="27"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="9">
-        <v>1</v>
+        <v>0.06</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="2">
@@ -1382,12 +2467,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="9">
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="2">
@@ -1400,12 +2485,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="9">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="2">
@@ -1418,11 +2503,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="21"/>
+      <c r="B31" s="21">
+        <f>SUM(B4:B30)</f>
+        <v>1</v>
+      </c>
       <c r="C31" s="22">
         <f>SUM(D4:D8,D10:D13,D15:D16,D18:D22,D24:D26,D28:D30)</f>
         <v>0</v>
@@ -1434,7 +2522,7 @@
       </c>
       <c r="F31" s="23"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="C31:D31"/>
@@ -1450,6 +2538,22 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3938CA-FD4E-254E-9C47-1BD64EA33416}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>